<commit_message>
Cập nhật mã nguồn với tính năng trắc nghiệm và từ vựng
</commit_message>
<xml_diff>
--- a/english_vocabulary.xlsx
+++ b/english_vocabulary.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HopTT\Desktop\Techtrage\CatalogSite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HopTT\Desktop\Techtrage\CatalogSite\tuvung_app\trantuanh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A46CA03F-C5D4-4B75-915B-0E0C33A1908E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668A3CBA-DF29-4B86-80DD-C75173F3F716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E31C756-6636-4A0E-A80B-19B20D540680}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lớp 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Unit1" sheetId="1" r:id="rId1"/>
+    <sheet name="Unit2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,78 +35,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
-  <si>
-    <t>Word</t>
-  </si>
-  <si>
-    <t>Meaning</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Example</t>
   </si>
   <si>
-    <t>Example_Vn</t>
-  </si>
-  <si>
-    <t>Grammar</t>
-  </si>
-  <si>
-    <t>Quiz</t>
-  </si>
-  <si>
-    <t>Reading_Text</t>
-  </si>
-  <si>
-    <t>Reading_Questions</t>
-  </si>
-  <si>
-    <t>Ball</t>
-  </si>
-  <si>
-    <t>A round object used for playing sports</t>
-  </si>
-  <si>
-    <t>I play with a ball every day.</t>
-  </si>
-  <si>
-    <t>Tôi chơi với quả bóng mỗi ngày.</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>[{"question": "What is the meaning of 'ball'?", "options": ["Quả bóng", "Xe đạp", "Sách"], "correct_answer": "Quả bóng"}]</t>
-  </si>
-  <si>
-    <t>"I play with a ball every day. It helps me stay healthy."</t>
-  </si>
-  <si>
-    <t>[{"question": "What does the person do with the ball?", "options": ["Play with it", "Eat it", "Throw it away"], "correct_answer": "Play with it"}]</t>
-  </si>
-  <si>
-    <t>Bike</t>
-  </si>
-  <si>
-    <t>A vehicle with two wheels that you ride by pushing pedals</t>
-  </si>
-  <si>
-    <t>I ride my bike to school.</t>
-  </si>
-  <si>
-    <t>Tôi đi xe đạp đến trường.</t>
-  </si>
-  <si>
-    <t>[{"question": "What is the correct sentence?", "options": ["I ride my bike to school.", "I ride my car to school.", "I ride my bus to school."], "correct_answer": "I ride my bike to school."}]</t>
-  </si>
-  <si>
-    <t>"I ride my bike to school every day. It's a short and fun journey."</t>
-  </si>
-  <si>
-    <t>[{"question": "How does the person get to school?", "options": ["By bike", "By car", "By bus"], "correct_answer": "By bike"}]</t>
-  </si>
-  <si>
-    <t>Unit</t>
+    <t>Vocabulary</t>
+  </si>
+  <si>
+    <t>IPA</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Reading Text</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>/ˈæpl/</t>
+  </si>
+  <si>
+    <t>I eat an apple every day.</t>
+  </si>
+  <si>
+    <t>"Apple" là một loại trái cây phổ biến.</t>
+  </si>
+  <si>
+    <t>"Apple" được dùng phổ biến trong tiếng Anh giao tiếp.</t>
+  </si>
+  <si>
+    <t>An apple a day keeps the doctor away.</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>/bʊk/</t>
+  </si>
+  <si>
+    <t>She reads a book every evening.</t>
+  </si>
+  <si>
+    <t>"Book" là vật phẩm để đọc.</t>
+  </si>
+  <si>
+    <t>Một cuốn sách có thể là một tài liệu học tập hoặc giải trí.</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Option 1</t>
+  </si>
+  <si>
+    <t>Option 2</t>
+  </si>
+  <si>
+    <t>Option 3</t>
+  </si>
+  <si>
+    <t>Correct Answer</t>
+  </si>
+  <si>
+    <t>What is the fruit you eat every day?</t>
+  </si>
+  <si>
+    <t>"Apple" is a fruit, you eat it every day.</t>
+  </si>
+  <si>
+    <t>Which object do you read every evening?</t>
+  </si>
+  <si>
+    <t>"Book" is an object that you can read.</t>
   </si>
 </sst>
 </file>
@@ -471,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4089CB8-5CE6-4BEB-AE43-4E7C70D49E10}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,98 +493,153 @@
     <col min="5" max="5" width="31.7109375" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" customWidth="1"/>
     <col min="7" max="7" width="30.5703125" customWidth="1"/>
-    <col min="8" max="8" width="37.85546875" customWidth="1"/>
-    <col min="9" max="9" width="75.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
+    <row r="3" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>22</v>
-      </c>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701A0A00-A9F6-464C-B01C-9B32E13CCEB0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>